<commit_message>
Uploaded Bama week 12 data
</commit_message>
<xml_diff>
--- a/school_colors/school_colors.xlsx
+++ b/school_colors/school_colors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="1257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="1262">
   <si>
     <t xml:space="preserve">School</t>
   </si>
@@ -3446,6 +3446,21 @@
   </si>
   <si>
     <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utah Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#BA1C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#003058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTAH TECH</t>
   </si>
   <si>
     <t xml:space="preserve">UTEP</t>
@@ -3801,7 +3816,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3836,6 +3851,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3880,7 +3901,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3903,6 +3924,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4014,13 +4039,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z248"/>
+  <dimension ref="A1:Z249"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F221" activeCellId="0" sqref="F221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.71"/>
@@ -13471,26 +13496,25 @@
         <v>1142</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>1022</v>
+        <v>1143</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>19</v>
+        <v>1144</v>
       </c>
       <c r="D221" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E221:Z221),")")</f>
-        <v>(UTEP|TEP|UTE)</v>
+        <v>(UTU|UTAH TECH|Utah)</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>1142</v>
-      </c>
-      <c r="F221" s="3" t="s">
-        <v>1143</v>
+        <v>1145</v>
+      </c>
+      <c r="F221" s="6" t="s">
+        <v>1146</v>
       </c>
       <c r="G221" s="3" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="H221" s="3"/>
-      <c r="I221" s="3"/>
       <c r="J221" s="3"/>
       <c r="K221" s="3"/>
       <c r="L221" s="3"/>
@@ -13511,30 +13535,29 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>1144</v>
+        <v>1147</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>37</v>
+        <v>1022</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>1145</v>
+        <v>19</v>
       </c>
       <c r="D222" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E222:Z222),")")</f>
-        <v>(VANDERBILT|VANDY|VAN|VU)</v>
+        <v>(UTEP|TEP|UTE)</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="F222" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>1148</v>
-      </c>
-      <c r="H222" s="3" t="s">
-        <v>1149</v>
-      </c>
+        <v>1135</v>
+      </c>
+      <c r="H222" s="3"/>
+      <c r="I222" s="3"/>
       <c r="J222" s="3"/>
       <c r="K222" s="3"/>
       <c r="L222" s="3"/>
@@ -13555,27 +13578,30 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C223" s="2" t="s">
         <v>1150</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>664</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>1151</v>
       </c>
       <c r="D223" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E223:Z223),")")</f>
-        <v>(VILLANOVA|VU)</v>
+        <v>(VANDERBILT|VANDY|VAN|VU)</v>
       </c>
       <c r="E223" s="3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F223" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="F223" s="3" t="s">
-        <v>1149</v>
-      </c>
-      <c r="G223" s="3"/>
-      <c r="H223" s="3"/>
-      <c r="I223" s="3"/>
+      <c r="G223" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H223" s="3" t="s">
+        <v>1154</v>
+      </c>
       <c r="J223" s="3"/>
       <c r="K223" s="3"/>
       <c r="L223" s="3"/>
@@ -13596,27 +13622,25 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>1154</v>
+        <v>664</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D224" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E224:Z224),")")</f>
-        <v>(VIRGINIA|VA|UVA)</v>
+        <v>(VILLANOVA|VU)</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>1157</v>
-      </c>
-      <c r="G224" s="3" t="s">
-        <v>1158</v>
-      </c>
+        <v>1154</v>
+      </c>
+      <c r="G224" s="3"/>
       <c r="H224" s="3"/>
       <c r="I224" s="3"/>
       <c r="J224" s="3"/>
@@ -13639,33 +13663,29 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>1159</v>
       </c>
-      <c r="B225" s="2" t="s">
+      <c r="C225" s="2" t="s">
         <v>1160</v>
-      </c>
-      <c r="C225" s="2" t="s">
-        <v>1161</v>
       </c>
       <c r="D225" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E225:Z225),")")</f>
-        <v>(VIRGINIA TECH|VATECH|VT|VaT|VAT)</v>
+        <v>(VIRGINIA|VA|UVA)</v>
       </c>
       <c r="E225" s="3" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F225" s="3" t="s">
         <v>1162</v>
       </c>
-      <c r="F225" s="3" t="s">
+      <c r="G225" s="3" t="s">
         <v>1163</v>
       </c>
-      <c r="G225" s="3" t="s">
-        <v>1164</v>
-      </c>
-      <c r="H225" s="3" t="s">
-        <v>1165</v>
-      </c>
-      <c r="I225" s="3" t="s">
-        <v>1166</v>
-      </c>
+      <c r="H225" s="3"/>
+      <c r="I225" s="3"/>
       <c r="J225" s="3"/>
       <c r="K225" s="3"/>
       <c r="L225" s="3"/>
@@ -13686,25 +13706,33 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>583</v>
+        <v>1166</v>
       </c>
       <c r="D226" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E226:Z226),")")</f>
-        <v>(VMI)</v>
+        <v>(VIRGINIA TECH|VATECH|VT|VaT|VAT)</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>1167</v>
       </c>
-      <c r="F226" s="3"/>
-      <c r="G226" s="3"/>
-      <c r="H226" s="3"/>
-      <c r="I226" s="3"/>
+      <c r="F226" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G226" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H226" s="3" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I226" s="3" t="s">
+        <v>1171</v>
+      </c>
       <c r="J226" s="3"/>
       <c r="K226" s="3"/>
       <c r="L226" s="3"/>
@@ -13725,24 +13753,22 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>1169</v>
+        <v>1172</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>1170</v>
+        <v>1173</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>1171</v>
+        <v>583</v>
       </c>
       <c r="D227" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E227:Z227),")")</f>
-        <v>(WAGNER|WAG)</v>
+        <v>(VMI)</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>1172</v>
       </c>
-      <c r="F227" s="3" t="s">
-        <v>1173</v>
-      </c>
+      <c r="F227" s="3"/>
       <c r="G227" s="3"/>
       <c r="H227" s="3"/>
       <c r="I227" s="3"/>
@@ -13772,24 +13798,20 @@
         <v>1175</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>37</v>
+        <v>1176</v>
       </c>
       <c r="D228" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E228:Z228),")")</f>
-        <v>(WAKE FOREST|WAKEFOREST|WFU|WF)</v>
+        <v>(WAGNER|WAG)</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G228" s="0" t="s">
         <v>1178</v>
       </c>
-      <c r="H228" s="3" t="s">
-        <v>1179</v>
-      </c>
+      <c r="G228" s="3"/>
+      <c r="H228" s="3"/>
       <c r="I228" s="3"/>
       <c r="J228" s="3"/>
       <c r="K228" s="3"/>
@@ -13811,33 +13833,31 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>1180</v>
       </c>
-      <c r="B229" s="2" t="s">
-        <v>1181</v>
-      </c>
       <c r="C229" s="2" t="s">
-        <v>1182</v>
+        <v>37</v>
       </c>
       <c r="D229" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E229:Z229),")")</f>
-        <v>(WASHINGTON|WASH|UW|WAS|U W)</v>
+        <v>(WAKE FOREST|WAKEFOREST|WFU|WF)</v>
       </c>
       <c r="E229" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F229" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G229" s="0" t="s">
         <v>1183</v>
       </c>
-      <c r="F229" s="3" t="s">
+      <c r="H229" s="3" t="s">
         <v>1184</v>
       </c>
-      <c r="G229" s="3" t="s">
-        <v>1185</v>
-      </c>
-      <c r="H229" s="3" t="s">
-        <v>1186</v>
-      </c>
-      <c r="I229" s="3" t="s">
-        <v>1187</v>
-      </c>
+      <c r="I229" s="3"/>
       <c r="J229" s="3"/>
       <c r="K229" s="3"/>
       <c r="L229" s="3"/>
@@ -13858,31 +13878,33 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="D230" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E230:Z230),")")</f>
-        <v>(WASHINGTON ST|WSU|WASHST|COU)</v>
+        <v>(WASHINGTON|WASH|UW|WAS|U W)</v>
       </c>
       <c r="E230" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F230" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="G230" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H230" s="3" t="s">
         <v>1191</v>
       </c>
-      <c r="F230" s="3" t="s">
+      <c r="I230" s="3" t="s">
         <v>1192</v>
       </c>
-      <c r="G230" s="3" t="s">
-        <v>1193</v>
-      </c>
-      <c r="H230" s="3" t="s">
-        <v>1194</v>
-      </c>
-      <c r="I230" s="3"/>
       <c r="J230" s="3"/>
       <c r="K230" s="3"/>
       <c r="L230" s="3"/>
@@ -13903,30 +13925,31 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C231" s="2" t="s">
         <v>1195</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>1197</v>
       </c>
       <c r="D231" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E231:Z231),")")</f>
-        <v>(WEBER ST|WEBERST|WEBER|WSU)</v>
+        <v>(WASHINGTON ST|WSU|WASHST|COU)</v>
       </c>
       <c r="E231" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="G231" s="3" t="s">
         <v>1198</v>
       </c>
-      <c r="F231" s="3" t="s">
+      <c r="H231" s="3" t="s">
         <v>1199</v>
       </c>
-      <c r="G231" s="3" t="s">
-        <v>1200</v>
-      </c>
-      <c r="H231" s="3" t="s">
-        <v>1192</v>
-      </c>
+      <c r="I231" s="3"/>
       <c r="J231" s="3"/>
       <c r="K231" s="3"/>
       <c r="L231" s="3"/>
@@ -13947,31 +13970,30 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B232" s="2" t="s">
         <v>1201</v>
       </c>
-      <c r="B232" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="C232" s="2" t="s">
-        <v>963</v>
+        <v>1202</v>
       </c>
       <c r="D232" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E232:Z232),")")</f>
-        <v>(WEST VIRGINIA|WESTVIR|WVU|WVirg)</v>
+        <v>(WEBER ST|WEBERST|WEBER|WSU)</v>
       </c>
       <c r="E232" s="3" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="G232" s="3" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="H232" s="3" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I232" s="3"/>
+        <v>1197</v>
+      </c>
       <c r="J232" s="3"/>
       <c r="K232" s="3"/>
       <c r="L232" s="3"/>
@@ -13995,26 +14017,26 @@
         <v>1206</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>1207</v>
+        <v>199</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>1208</v>
+        <v>963</v>
       </c>
       <c r="D233" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E233:Z233),")")</f>
-        <v>(WESTERN CAROLINA|WESTCARLNA|WESTRN CAROLINA|WCU)</v>
+        <v>(WEST VIRGINIA|WESTVIR|WVU|WVirg)</v>
       </c>
       <c r="E233" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F233" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G233" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="F233" s="3" t="s">
+      <c r="H233" s="3" t="s">
         <v>1210</v>
-      </c>
-      <c r="G233" s="3" t="s">
-        <v>1211</v>
-      </c>
-      <c r="H233" s="3" t="s">
-        <v>1212</v>
       </c>
       <c r="I233" s="3"/>
       <c r="J233" s="3"/>
@@ -14037,26 +14059,30 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C234" s="2" t="s">
         <v>1213</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D234" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E234:Z234),")")</f>
-        <v>(WESTRN ILLINOIS|WIU)</v>
+        <v>(WESTERN CAROLINA|WESTCARLNA|WESTRN CAROLINA|WCU)</v>
       </c>
       <c r="E234" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F234" s="3" t="s">
         <v>1215</v>
       </c>
-      <c r="F234" s="3" t="s">
+      <c r="G234" s="3" t="s">
         <v>1216</v>
       </c>
-      <c r="G234" s="3"/>
-      <c r="H234" s="3"/>
+      <c r="H234" s="3" t="s">
+        <v>1217</v>
+      </c>
       <c r="I234" s="3"/>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
@@ -14078,27 +14104,25 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>382</v>
+        <v>1219</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>1218</v>
+        <v>55</v>
       </c>
       <c r="D235" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E235:Z235),")")</f>
-        <v>(WESTRN KENTUCKY|WKU|WESTERNKY)</v>
+        <v>(WESTRN ILLINOIS|WIU)</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="F235" s="3" t="s">
-        <v>1220</v>
-      </c>
-      <c r="G235" s="3" t="s">
         <v>1221</v>
       </c>
+      <c r="G235" s="3"/>
       <c r="H235" s="3"/>
       <c r="I235" s="3"/>
       <c r="J235" s="3"/>
@@ -14124,27 +14148,25 @@
         <v>1222</v>
       </c>
       <c r="B236" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C236" s="2" t="s">
         <v>1223</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>1224</v>
       </c>
       <c r="D236" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E236:Z236),")")</f>
-        <v>(WESTMICH|WESTRN MICHIGAN|WMU|WMI)</v>
+        <v>(WESTRN KENTUCKY|WKU|WESTERNKY)</v>
       </c>
       <c r="E236" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F236" s="3" t="s">
         <v>1225</v>
       </c>
-      <c r="F236" s="3" t="s">
+      <c r="G236" s="3" t="s">
         <v>1226</v>
       </c>
-      <c r="G236" s="3" t="s">
-        <v>1227</v>
-      </c>
-      <c r="H236" s="3" t="s">
-        <v>1228</v>
-      </c>
+      <c r="H236" s="3"/>
       <c r="I236" s="3"/>
       <c r="J236" s="3"/>
       <c r="K236" s="3"/>
@@ -14166,28 +14188,30 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C237" s="2" t="s">
         <v>1229</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>1231</v>
       </c>
       <c r="D237" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E237:Z237),")")</f>
-        <v>(MARY|WILLMMARY|WM)</v>
+        <v>(WESTMICH|WESTRN MICHIGAN|WMU|WMI)</v>
       </c>
       <c r="E237" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="G237" s="3" t="s">
         <v>1232</v>
       </c>
-      <c r="F237" s="0" t="s">
+      <c r="H237" s="3" t="s">
         <v>1233</v>
       </c>
-      <c r="G237" s="3" t="s">
-        <v>1234</v>
-      </c>
-      <c r="H237" s="3"/>
       <c r="I237" s="3"/>
       <c r="J237" s="3"/>
       <c r="K237" s="3"/>
@@ -14209,25 +14233,27 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B238" s="2" t="s">
         <v>1235</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="C238" s="2" t="s">
         <v>1236</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D238" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E238:Z238),")")</f>
-        <v>(WISCONSIN|WIS)</v>
+        <v>(MARY|WILLMMARY|WM)</v>
       </c>
       <c r="E238" s="3" t="s">
         <v>1237</v>
       </c>
-      <c r="F238" s="3" t="s">
+      <c r="F238" s="0" t="s">
         <v>1238</v>
       </c>
-      <c r="G238" s="3"/>
+      <c r="G238" s="3" t="s">
+        <v>1239</v>
+      </c>
       <c r="H238" s="3"/>
       <c r="I238" s="3"/>
       <c r="J238" s="3"/>
@@ -14250,23 +14276,23 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D239" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E239:Z239),")")</f>
-        <v>(WOFFORD|WOF)</v>
+        <v>(WISCONSIN|WIS)</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="F239" s="3" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="G239" s="3"/>
       <c r="H239" s="3"/>
@@ -14291,17 +14317,17 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>1245</v>
+        <v>31</v>
       </c>
       <c r="D240" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E240:Z240),")")</f>
-        <v>(WYOMING|WYO|WY)</v>
+        <v>(WOFFORD|WOF)</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>1246</v>
@@ -14309,9 +14335,9 @@
       <c r="F240" s="3" t="s">
         <v>1247</v>
       </c>
-      <c r="G240" s="3" t="s">
-        <v>1248</v>
-      </c>
+      <c r="G240" s="3"/>
+      <c r="H240" s="3"/>
+      <c r="I240" s="3"/>
       <c r="J240" s="3"/>
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
@@ -14332,17 +14358,17 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B241" s="2" t="s">
         <v>1249</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="C241" s="2" t="s">
         <v>1250</v>
-      </c>
-      <c r="C241" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D241" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E241:Z241),")")</f>
-        <v>(YALE|YAL)</v>
+        <v>(WYOMING|WYO|WY)</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>1251</v>
@@ -14350,9 +14376,9 @@
       <c r="F241" s="3" t="s">
         <v>1252</v>
       </c>
-      <c r="G241" s="3"/>
-      <c r="H241" s="3"/>
-      <c r="I241" s="3"/>
+      <c r="G241" s="3" t="s">
+        <v>1253</v>
+      </c>
       <c r="J241" s="3"/>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -14373,23 +14399,23 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>415</v>
+        <v>1255</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>1254</v>
+        <v>31</v>
       </c>
       <c r="D242" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E242:Z242),")")</f>
-        <v>(YOUNGSTOWN ST|YSU)</v>
+        <v>(YALE|YAL)</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="F242" s="3" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="G242" s="3"/>
       <c r="H242" s="3"/>
@@ -14413,8 +14439,25 @@
       <c r="Z242" s="3"/>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E243" s="3"/>
-      <c r="F243" s="3"/>
+      <c r="A243" s="0" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D243" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E243:Z243),")")</f>
+        <v>(YOUNGSTOWN ST|YSU)</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>1261</v>
+      </c>
       <c r="G243" s="3"/>
       <c r="H243" s="3"/>
       <c r="I243" s="3"/>
@@ -14556,14 +14599,38 @@
       <c r="Y248" s="3"/>
       <c r="Z248" s="3"/>
     </row>
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="3"/>
+      <c r="H249" s="3"/>
+      <c r="I249" s="3"/>
+      <c r="J249" s="3"/>
+      <c r="K249" s="3"/>
+      <c r="L249" s="3"/>
+      <c r="M249" s="3"/>
+      <c r="N249" s="3"/>
+      <c r="O249" s="3"/>
+      <c r="P249" s="3"/>
+      <c r="Q249" s="3"/>
+      <c r="R249" s="3"/>
+      <c r="S249" s="3"/>
+      <c r="T249" s="3"/>
+      <c r="U249" s="3"/>
+      <c r="V249" s="3"/>
+      <c r="W249" s="3"/>
+      <c r="X249" s="3"/>
+      <c r="Y249" s="3"/>
+      <c r="Z249" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A194:A1048576 A77:A192 A1:A75">
+  <conditionalFormatting sqref="A222:A1048576 A77:A192 A1:A75 A194:A220">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J124:Z124 E124:H124 E125:Z126 E2:Z2 E58:Z58 H56:Z57 E56:F56 E57:G57 E59:H59 J59:Z59 E60:Z62 H64:Z64 E64:F64 F65:Z66 E65:E70 F72:Z73 I70:Z70 F70:G70 H71:Z71 E71:F71 E72:E74 E75:Z76 I74:Z74 F74:G74 E79:Z90 E77:G77 I77:Z77 E96:Z99 H95:Z95 E94:F95 E102:Z104 E101:G101 I101:Z101 E107:Z107 H106:Z106 E106:F106 H109:Z109 E108:E109 E110:Z114 E118:Z123 E116:H116 J115:Z116 E115:G117 I117:Z117 E129:Z131 H128:Z128 E128:F128 E134:Z145 E132:F132 H132:Z132 F149:Z161 E146:I146 L146:Z146 E166:Z167 E165:G165 I165:Z165 E169:Z171 I168:Z168 E168:G168 E173:Z183 E172:J172 N172:Z172 E185:Z188 J184:Z184 E184:H184 E189:H189 K189:Z189 E197:Z198 I195:Z196 E195:G196 E201:Z201 I199:Z199 E199:G199 E200:H200 J200:Z200 E203:Z203 E202:I202 K202:Z202 E208:Z214 E207:G207 I207:Z207 E3:H3 J3:Z3 I115 E4:Z9 E10:F10 H10:Z10 E41:Z47 E40:F40 H40:Z40 E92:Z93 E91:F91 H91:Z91 E24:Z35 E23 G23:Z23 E147:E162 E163:Z163 G162:Z162 F105:Z105 E206:Z206 E204:F205 H204:Z205 E127 G127:Z127 F68:Z69 F67:G67 I67:Z67 E50:Z55 E48 G48:Z48 M100:Z100 E100:F101 I100:K100 G100 E78 G78:Z78 F190:Z190 G108:Z108 K147:Z147 H147:I148 F147:F148 E133:I133 K133:Z133 F49:Z49 E37:Z39 E36 G36:Z36 J148:Z148 E63:G63 I63:Z63 J94:Z94 G94:H94 E11:Z22 E164 G164:Z164 E191:Z194">
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E216:Z219 E221:Z221 E220:H220 J220:Z220 E223:Z227 E222:H222 J222:Z222 E232:Z236 E231:H231 J231:Z231 E241:Z248 J240:Z240 E240:G240 E229:Z230 E228:F228 H228:Z228 G215:Z215 E215 E238:Z239 E237 G237:Z237">
+  <conditionalFormatting sqref="E216:Z219 E222:Z222 E220:H220 J220:Z221 E224:Z228 E223:H223 J223:Z223 E233:Z237 E232:H232 J232:Z232 E242:Z249 J241:Z241 E241:G241 E230:Z231 E229:F229 H229:Z229 G215:Z215 E215 E239:Z240 E238 G238:Z238 E221 G221:H221">
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed penalties, upload game
</commit_message>
<xml_diff>
--- a/school_colors/school_colors.xlsx
+++ b/school_colors/school_colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\program_project\CFB\school_colors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A230088F-240A-457F-80F8-3AF9374EF182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FA8166-9D2A-40D5-96DC-07F5C6AE4255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="5670" windowWidth="25440" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="school_colors" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="1375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="1375">
   <si>
     <t>School</t>
   </si>
@@ -4632,8 +4632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>(ALABAMA|ALA|Alab|UA)</v>
+        <v>(ALABAMA|ALA|Alabama|Alab|UA)</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -4759,9 +4759,12 @@
         <v>27</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -10907,7 +10910,7 @@
   <conditionalFormatting sqref="E216:Z218 G219:Z219 E219 E222:Z222 E220:H220 J220:Z221 E225:Z225 E228:Z229 E227:F227 H227:Z227 G226:Z226 E226 E224:F224 H224:Z224 E234:Z234 E236:Z237 E238:G238 I238:Z238 E235:G235 I235:Z235 E233:H233 J233:Z233 E243:Z250 J242:Z242 E242 G242:H242 E232:Z232 H230:Z231 E230:F231 G215:Z215 E215 E241:Z241 G239:Z240 E239:E240 E221 G221:H221 F223:Z223">
     <cfRule type="duplicateValues" dxfId="1" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I109 H100:J100 J124:Z124 E124:H124 E125:Z125 G127:Z127 I126:Z126 F126:G126 E2:Z2 E58:Z58 E56:F57 H56:Z56 K57:Z57 G57:I57 E59:H59 J59:Z59 E60:Z62 H64:Z64 E64:F64 F65:Z66 E65:E70 F72:Z73 I70:Z70 F70:G70 H71:Z71 E71:F71 E72:E74 E75:Z76 J74:Z74 F74:H74 E79:Z79 E81:Z89 G80:Z80 E80 K91:Z91 H91:I91 L90:Z90 G90:J90 E77:G77 I77:Z77 E96:Z99 H95:Z95 E94:F95 E103:Z104 K102:Z102 E102:I102 I101:Z101 E107:Z107 H106:Z106 E106:F106 E108:E109 E110:Z110 E113:Z114 E112:G112 I112:Z112 E111:H111 J111:Z111 E118:Z118 E120:Z122 E123:F123 H123:Z123 J119:Z119 E119:H119 E115:G116 J115:Z116 J117:K117 M117:Z117 E116:H117 E130:Z130 K131:Z131 E131:I131 G129:I129 K129:Z129 E128:F129 H128:Z128 E134:Z137 E139:Z145 G138:Z138 E138 E132:G132 F152:Z153 J151:Z151 F151:H151 L150:Z150 F150:J150 G149:H149 J149:Z149 F156:Z161 I155:Z155 F155:G155 L154:Z154 F154:J154 E146:I146 L146:Z146 E166:Z166 I168:Z168 J167:Z167 E165:G165 I165:Z165 E169:Z171 E168:G168 E167:H167 E174:Z176 E173:F173 H173:Z173 E179:Z181 E183:Z183 J182:Z182 E182:H182 E177:F178 E172:G172 I172:K172 N172:Z172 E185:Z188 J184:Z184 E184:H184 E189 G189:I189 K189:Z189 E197:Z197 G198:Z199 G195:Z195 J196:Z196 F196:H196 E195:E196 E201:Z201 E198:E199 E200:F200 H200:Z200 E203:Z203 E202:F202 H202:Z202 E208:Z208 E210:Z210 E212:Z213 E214:F214 H214:Z214 G211:Z211 E211 G209:Z209 E209 E207:G207 I207:Z207 E3:H3 J3:Z3 I115 E4:Z4 E10:F10 I10:Z10 E92:Z93 E90:F91 E23 G23:Z23 E147:E162 E163:Z163 G162:Z162 F105:Z105 E206:Z206 E204:F204 E205 G205 H204:Z204 I205:Z205 E126:E127 F68:Z68 L69:Z69 F69:J69 F67:G67 I67:Z67 E50:Z53 E55:Z55 E54:F54 H54:Z54 E48 G48:Z48 E101:G101 N100:Z100 L100 E100:F100 J78:Z78 E78:F78 H78 F190:Z190 J108:Z108 K109:Z109 F109 G108:H108 K147:Z147 H147:I147 F147:F149 E133:I133 K133:Z133 F49:Z49 E37:Z37 E39:F40 H39:Z40 G38:Z38 E38 E36 G36:Z36 L148:Z148 H148:J148 E63:G63 I63:Z63 J94:Z94 G94:H94 E11:Z11 E13:Z13 E12:F12 H12:Z12 E15:Z15 G16:Z16 E16 E14:F14 H14:Z14 E164 G164:Z164 E191:Z194 E6:Z9 E5 G5:Z5 L132:Z132 I132:J132 E18:Z18 E20:Z21 E22:F22 H22:Z22 E19:G19 I19:Z19 E17:F17 H17:Z17 E24:Z28 E30:Z33 G29:Z29 E29 E35:Z35 E34:F34 H34:Z34 E41:Z42 E45:Z47 H43:Z44 E43:F44 H177:Z178">
+  <conditionalFormatting sqref="I109 H100:J100 J124:Z124 E124:H124 E125:Z125 G127:Z127 I126:Z126 F126:G126 E2:Z2 E58:Z58 E56:F57 H56:Z56 K57:Z57 G57:I57 E59:H59 J59:Z59 E60:Z62 H64:Z64 E64:F64 F65:Z66 E65:E70 F72:Z73 I70:Z70 F70:G70 H71:Z71 E71:F71 E72:E74 E75:Z76 J74:Z74 F74:H74 E79:Z79 E81:Z89 G80:Z80 E80 K91:Z91 H91:I91 L90:Z90 G90:J90 E77:G77 I77:Z77 E96:Z99 H95:Z95 E94:F95 E103:Z104 K102:Z102 E102:I102 I101:Z101 E107:Z107 H106:Z106 E106:F106 E108:E109 E110:Z110 E113:Z114 E112:G112 I112:Z112 E111:H111 J111:Z111 E118:Z118 E120:Z122 E123:F123 H123:Z123 J119:Z119 E119:H119 E115:G116 J115:Z116 J117:K117 M117:Z117 E116:H117 E130:Z130 K131:Z131 E131:I131 G129:I129 K129:Z129 E128:F129 H128:Z128 E134:Z137 E139:Z145 G138:Z138 E138 E132:G132 F152:Z153 J151:Z151 F151:H151 L150:Z150 F150:J150 G149:H149 J149:Z149 F156:Z161 I155:Z155 F155:G155 L154:Z154 F154:J154 E146:I146 L146:Z146 E166:Z166 I168:Z168 J167:Z167 E165:G165 I165:Z165 E169:Z171 E168:G168 E167:H167 E174:Z176 E173:F173 H173:Z173 E179:Z181 E183:Z183 J182:Z182 E182:H182 E177:F178 E172:G172 I172:K172 N172:Z172 E185:Z188 J184:Z184 E184:H184 E189 G189:I189 K189:Z189 E197:Z197 G198:Z199 G195:Z195 J196:Z196 F196:H196 E195:E196 E201:Z201 E198:E199 E200:F200 H200:Z200 E203:Z203 E202:F202 H202:Z202 E208:Z208 E210:Z210 E212:Z213 E214:F214 H214:Z214 G211:Z211 E211 G209:Z209 E209 E207:G207 I207:Z207 E3:H3 J3:Z3 I115 E4:Z4 E10:F10 I10:Z10 E92:Z93 E90:F91 E23 G23:Z23 E147:E162 E163:Z163 G162:Z162 F105:Z105 E206:Z206 E204:F204 E205 G205 H204:Z204 I205:Z205 E126:E127 F68:Z68 L69:Z69 F69:J69 F67:G67 I67:Z67 E50:Z53 E55:Z55 E54:F54 H54:Z54 E48 G48:Z48 E101:G101 N100:Z100 L100 E100:F100 J78:Z78 E78:F78 H78 F190:Z190 J108:Z108 K109:Z109 F109 G108:H108 K147:Z147 H147:I147 F147:F149 E133:I133 K133:Z133 F49:Z49 E37:Z37 E39:F40 H39:Z40 G38:Z38 E38 E36 G36:Z36 L148:Z148 H148:J148 E63:G63 I63:Z63 J94:Z94 G94:H94 E11:Z11 E13:Z13 E12:F12 H12:Z12 E15:Z15 G16:Z16 E16 E14:F14 H14:Z14 E164 G164:Z164 E191:Z194 E6:Z9 E5 L132:Z132 I132:J132 E18:Z18 E20:Z21 E22:F22 H22:Z22 E19:G19 I19:Z19 E17:F17 H17:Z17 E24:Z28 E30:Z33 G29:Z29 E29 E35:Z35 E34:F34 H34:Z34 E41:Z42 E45:Z47 H43:Z44 E43:F44 H177:Z178 G5:Z5">
     <cfRule type="duplicateValues" dxfId="0" priority="19"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
New game data, etc.
</commit_message>
<xml_diff>
--- a/school_colors/school_colors.xlsx
+++ b/school_colors/school_colors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="1375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="1380">
   <si>
     <t xml:space="preserve">School</t>
   </si>
@@ -2845,6 +2845,9 @@
     <t xml:space="preserve">RCE</t>
   </si>
   <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Richmond</t>
   </si>
   <si>
@@ -2887,9 +2890,6 @@
     <t xml:space="preserve">RUT</t>
   </si>
   <si>
-    <t xml:space="preserve">RU</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sacramento State</t>
   </si>
   <si>
@@ -3425,6 +3425,21 @@
   </si>
   <si>
     <t xml:space="preserve">TAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas A&amp;M-Commerce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#1D2953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#E8A311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAMC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXCC</t>
   </si>
   <si>
     <t xml:space="preserve">Texas Southern</t>
@@ -4155,7 +4170,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4188,6 +4203,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -4234,7 +4257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4257,6 +4280,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4368,20 +4395,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z250"/>
+  <dimension ref="A1:Z251"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G181" activeCellId="0" sqref="G181"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I165" activeCellId="0" sqref="I165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.71"/>
@@ -11543,7 +11570,7 @@
       </c>
       <c r="D164" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E164:Z164),")")</f>
-        <v>(RICE|Rice|RIC|RCE)</v>
+        <v>(RICE|Rice|RIC|RCE|RU)</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>938</v>
@@ -11557,7 +11584,9 @@
       <c r="H164" s="3" t="s">
         <v>940</v>
       </c>
-      <c r="I164" s="3"/>
+      <c r="I164" s="3" t="s">
+        <v>941</v>
+      </c>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
       <c r="L164" s="3"/>
@@ -11578,10 +11607,10 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>490</v>
@@ -11591,13 +11620,13 @@
         <v>(RICHMOND|RIC|UR)</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="F165" s="3" t="s">
         <v>939</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
@@ -11620,23 +11649,23 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="D166" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E166:Z166),")")</f>
         <v>(RMU|ROBERT MORRIS)</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
@@ -11661,29 +11690,29 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="D167" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E167:Z167),")")</f>
         <v>(RUTGERS|Rutgr|RUT|RU)</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="H167" s="3" t="s">
-        <v>955</v>
+        <v>941</v>
       </c>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
@@ -11875,7 +11904,7 @@
         <v>977</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>38</v>
@@ -13143,32 +13172,30 @@
       <c r="Y200" s="3"/>
       <c r="Z200" s="3"/>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="3" t="s">
         <v>1135</v>
       </c>
-      <c r="B201" s="2" t="s">
+      <c r="B201" s="6" t="s">
         <v>1136</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="C201" s="6" t="s">
         <v>1137</v>
       </c>
       <c r="D201" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E201:Z201),")")</f>
-        <v>(TEXAS SOUTHERN|TSU|TXSOFB|TexSo)</v>
+        <v>(Texas A&amp;M-Commerce|TAMC|TXCC)</v>
       </c>
       <c r="E201" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F201" s="3" t="s">
         <v>1138</v>
       </c>
-      <c r="F201" s="3" t="s">
-        <v>1116</v>
-      </c>
-      <c r="G201" s="3" t="s">
+      <c r="G201" s="0" t="s">
         <v>1139</v>
       </c>
-      <c r="H201" s="3" t="s">
-        <v>1140</v>
-      </c>
+      <c r="H201" s="3"/>
       <c r="I201" s="3"/>
       <c r="J201" s="3"/>
       <c r="K201" s="3"/>
@@ -13190,36 +13217,32 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B202" s="2" t="s">
         <v>1141</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="C202" s="2" t="s">
         <v>1142</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>1143</v>
       </c>
       <c r="D202" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E202:Z202),")")</f>
-        <v>(TEXAS STATE|TEXSTATE|TexSt|TSU|TXST|TXS)</v>
+        <v>(TEXAS SOUTHERN|TSU|TXSOFB|TexSo)</v>
       </c>
       <c r="E202" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G202" s="3" t="s">
         <v>1144</v>
       </c>
-      <c r="F202" s="3" t="s">
+      <c r="H202" s="3" t="s">
         <v>1145</v>
       </c>
-      <c r="G202" s="0" t="s">
-        <v>1146</v>
-      </c>
-      <c r="H202" s="3" t="s">
-        <v>1116</v>
-      </c>
-      <c r="I202" s="3" t="s">
-        <v>1147</v>
-      </c>
-      <c r="J202" s="3" t="s">
-        <v>1148</v>
-      </c>
+      <c r="I202" s="3"/>
+      <c r="J202" s="3"/>
       <c r="K202" s="3"/>
       <c r="L202" s="3"/>
       <c r="M202" s="3"/>
@@ -13239,34 +13262,36 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>351</v>
+        <v>1147</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>38</v>
+        <v>1148</v>
       </c>
       <c r="D203" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E203:Z203),")")</f>
-        <v>(TEXAS TECH|TTU|TEXTC|TEXASTECH|TexTc)</v>
+        <v>(TEXAS STATE|TEXSTATE|TexSt|TSU|TXST|TXS)</v>
       </c>
       <c r="E203" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F203" s="3" t="s">
         <v>1150</v>
       </c>
-      <c r="F203" s="3" t="s">
-        <v>1122</v>
-      </c>
-      <c r="G203" s="3" t="s">
+      <c r="G203" s="0" t="s">
         <v>1151</v>
       </c>
       <c r="H203" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="I203" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="I203" s="3" t="s">
+      <c r="J203" s="3" t="s">
         <v>1153</v>
       </c>
-      <c r="J203" s="3"/>
       <c r="K203" s="3"/>
       <c r="L203" s="3"/>
       <c r="M203" s="3"/>
@@ -13289,26 +13314,30 @@
         <v>1154</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>1155</v>
+        <v>351</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>1156</v>
+        <v>38</v>
       </c>
       <c r="D204" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E204:Z204),")")</f>
-        <v>(CIT|THE CITADEL|THECITADEL)</v>
+        <v>(TEXAS TECH|TTU|TEXTC|TEXASTECH|TexTc)</v>
       </c>
       <c r="E204" s="3" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="H204" s="3" t="s">
         <v>1157</v>
       </c>
-      <c r="F204" s="3" t="s">
+      <c r="I204" s="3" t="s">
         <v>1158</v>
       </c>
-      <c r="G204" s="0" t="s">
-        <v>1159</v>
-      </c>
-      <c r="H204" s="3"/>
-      <c r="I204" s="3"/>
       <c r="J204" s="3"/>
       <c r="K204" s="3"/>
       <c r="L204" s="3"/>
@@ -13329,33 +13358,29 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>1160</v>
       </c>
-      <c r="B205" s="2" t="s">
+      <c r="C205" s="2" t="s">
         <v>1161</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>1162</v>
       </c>
       <c r="D205" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E205:Z205),")")</f>
-        <v>(TOLEDO|Toled|TOL|UTo|UT)</v>
+        <v>(CIT|THE CITADEL|THECITADEL)</v>
       </c>
       <c r="E205" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F205" s="3" t="s">
         <v>1163</v>
       </c>
-      <c r="F205" s="0" t="s">
+      <c r="G205" s="0" t="s">
         <v>1164</v>
       </c>
-      <c r="G205" s="3" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H205" s="0" t="s">
-        <v>1166</v>
-      </c>
-      <c r="I205" s="3" t="s">
-        <v>1113</v>
-      </c>
+      <c r="H205" s="3"/>
+      <c r="I205" s="3"/>
       <c r="J205" s="3"/>
       <c r="K205" s="3"/>
       <c r="L205" s="3"/>
@@ -13376,27 +13401,33 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>1167</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>1168</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>1169</v>
       </c>
       <c r="D206" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E206:Z206),")")</f>
-        <v>(TOWSON|TOW)</v>
+        <v>(TOLEDO|Toled|TOL|UTo|UT)</v>
       </c>
       <c r="E206" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F206" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G206" s="3" t="s">
         <v>1170</v>
       </c>
-      <c r="F206" s="3" t="s">
+      <c r="H206" s="0" t="s">
         <v>1171</v>
       </c>
-      <c r="G206" s="3"/>
-      <c r="H206" s="3"/>
-      <c r="I206" s="3"/>
+      <c r="I206" s="3" t="s">
+        <v>1113</v>
+      </c>
       <c r="J206" s="3"/>
       <c r="K206" s="3"/>
       <c r="L206" s="3"/>
@@ -13427,7 +13458,7 @@
       </c>
       <c r="D207" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E207:Z207),")")</f>
-        <v>(TROY|TRO|TRY)</v>
+        <v>(TOWSON|TOW)</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>1175</v>
@@ -13435,9 +13466,8 @@
       <c r="F207" s="3" t="s">
         <v>1176</v>
       </c>
-      <c r="G207" s="3" t="s">
-        <v>1177</v>
-      </c>
+      <c r="G207" s="3"/>
+      <c r="H207" s="3"/>
       <c r="I207" s="3"/>
       <c r="J207" s="3"/>
       <c r="K207" s="3"/>
@@ -13459,17 +13489,17 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>1178</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>1030</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>1179</v>
       </c>
       <c r="D208" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E208:Z208),")")</f>
-        <v>(TLN|TULANE|Tulan)</v>
+        <v>(TROY|TRO|TRY)</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>1180</v>
@@ -13480,7 +13510,6 @@
       <c r="G208" s="3" t="s">
         <v>1182</v>
       </c>
-      <c r="H208" s="3"/>
       <c r="I208" s="3"/>
       <c r="J208" s="3"/>
       <c r="K208" s="3"/>
@@ -13505,30 +13534,26 @@
         <v>1183</v>
       </c>
       <c r="B209" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>1184</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="D209" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E209:Z209),")")</f>
-        <v>(TULSA|Tulsa|TLS|Tul|TUL)</v>
+        <v>(TLN|TULANE|Tulan)</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>1185</v>
       </c>
-      <c r="F209" s="0" t="s">
-        <v>1183</v>
+      <c r="F209" s="3" t="s">
+        <v>1186</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>1186</v>
-      </c>
-      <c r="H209" s="3" t="s">
         <v>1187</v>
       </c>
-      <c r="I209" s="3" t="s">
-        <v>1188</v>
-      </c>
+      <c r="H209" s="3"/>
+      <c r="I209" s="3"/>
       <c r="J209" s="3"/>
       <c r="K209" s="3"/>
       <c r="L209" s="3"/>
@@ -13549,25 +13574,33 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B210" s="2" t="s">
         <v>1189</v>
       </c>
-      <c r="B210" s="2" t="s">
-        <v>1042</v>
-      </c>
       <c r="C210" s="2" t="s">
-        <v>1190</v>
+        <v>442</v>
       </c>
       <c r="D210" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E210:Z210),")")</f>
-        <v>(UAB)</v>
+        <v>(TULSA|Tulsa|TLS|Tul|TUL)</v>
       </c>
       <c r="E210" s="3" t="s">
-        <v>1189</v>
-      </c>
-      <c r="F210" s="3"/>
-      <c r="G210" s="3"/>
-      <c r="H210" s="3"/>
-      <c r="I210" s="3"/>
+        <v>1190</v>
+      </c>
+      <c r="F210" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="H210" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="I210" s="3" t="s">
+        <v>1193</v>
+      </c>
       <c r="J210" s="3"/>
       <c r="K210" s="3"/>
       <c r="L210" s="3"/>
@@ -13588,27 +13621,23 @@
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>1191</v>
+        <v>1194</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>214</v>
+        <v>1042</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>414</v>
+        <v>1195</v>
       </c>
       <c r="D211" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E211:Z211),")")</f>
-        <v>(UC DAVIS|UCDav|UCD)</v>
+        <v>(UAB)</v>
       </c>
       <c r="E211" s="3" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F211" s="0" t="s">
-        <v>1193</v>
-      </c>
-      <c r="G211" s="3" t="s">
         <v>1194</v>
       </c>
+      <c r="F211" s="3"/>
+      <c r="G211" s="3"/>
       <c r="H211" s="3"/>
       <c r="I211" s="3"/>
       <c r="J211" s="3"/>
@@ -13631,23 +13660,27 @@
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>1196</v>
+        <v>214</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>38</v>
+        <v>414</v>
       </c>
       <c r="D212" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E212:Z212),")")</f>
-        <v>(UCF)</v>
+        <v>(UC DAVIS|UCDav|UCD)</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F212" s="3"/>
-      <c r="G212" s="3"/>
+        <v>1197</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>1199</v>
+      </c>
       <c r="H212" s="3"/>
       <c r="I212" s="3"/>
       <c r="J212" s="3"/>
@@ -13670,24 +13703,22 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>1198</v>
+        <v>1201</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="D213" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E213:Z213),")")</f>
-        <v>(UCLA|UCL)</v>
+        <v>(UCF)</v>
       </c>
       <c r="E213" s="3" t="s">
-        <v>1197</v>
-      </c>
-      <c r="F213" s="3" t="s">
-        <v>1199</v>
-      </c>
+        <v>1200</v>
+      </c>
+      <c r="F213" s="3"/>
       <c r="G213" s="3"/>
       <c r="H213" s="3"/>
       <c r="I213" s="3"/>
@@ -13711,33 +13742,27 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>1202</v>
+        <v>129</v>
       </c>
       <c r="D214" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E214:Z214),")")</f>
-        <v>(MASSACHUSETTS|UMASS|UMass|UMA|MAS)</v>
+        <v>(UCLA|UCL)</v>
       </c>
       <c r="E214" s="3" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F214" s="3" t="s">
         <v>1204</v>
       </c>
-      <c r="G214" s="0" t="s">
-        <v>1200</v>
-      </c>
-      <c r="H214" s="3" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I214" s="3" t="s">
-        <v>1206</v>
-      </c>
+      <c r="G214" s="3"/>
+      <c r="H214" s="3"/>
+      <c r="I214" s="3"/>
       <c r="J214" s="3"/>
       <c r="K214" s="3"/>
       <c r="L214" s="3"/>
@@ -13758,29 +13783,33 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C215" s="2" t="s">
         <v>1207</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>1209</v>
       </c>
       <c r="D215" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E215:Z215),")")</f>
-        <v>(LV|NLV|UNLV)</v>
+        <v>(MASSACHUSETTS|UMASS|UMass|UMA|MAS)</v>
       </c>
       <c r="E215" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F215" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G215" s="0" t="s">
+        <v>1205</v>
+      </c>
+      <c r="H215" s="3" t="s">
         <v>1210</v>
       </c>
-      <c r="F215" s="0" t="s">
+      <c r="I215" s="3" t="s">
         <v>1211</v>
       </c>
-      <c r="G215" s="3" t="s">
-        <v>1207</v>
-      </c>
-      <c r="H215" s="3"/>
-      <c r="I215" s="3"/>
       <c r="J215" s="3"/>
       <c r="K215" s="3"/>
       <c r="L215" s="3"/>
@@ -13801,23 +13830,27 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>1010</v>
+        <v>1212</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>490</v>
+        <v>1213</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>305</v>
+        <v>1214</v>
       </c>
       <c r="D216" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E216:Z216),")")</f>
-        <v>(USC)</v>
+        <v>(LV|NLV|UNLV)</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F216" s="3"/>
-      <c r="G216" s="3"/>
+        <v>1215</v>
+      </c>
+      <c r="F216" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G216" s="3" t="s">
+        <v>1212</v>
+      </c>
       <c r="H216" s="3"/>
       <c r="I216" s="3"/>
       <c r="J216" s="3"/>
@@ -13840,27 +13873,23 @@
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>1212</v>
+        <v>1010</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>1213</v>
+        <v>490</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>1214</v>
+        <v>305</v>
       </c>
       <c r="D217" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E217:Z217),")")</f>
-        <v>(TENN MARTIN|UTM|TENNMARTIN)</v>
+        <v>(USC)</v>
       </c>
       <c r="E217" s="3" t="s">
-        <v>1215</v>
-      </c>
-      <c r="F217" s="3" t="s">
-        <v>1216</v>
-      </c>
-      <c r="G217" s="3" t="s">
-        <v>1217</v>
-      </c>
+        <v>1010</v>
+      </c>
+      <c r="F217" s="3"/>
+      <c r="G217" s="3"/>
       <c r="H217" s="3"/>
       <c r="I217" s="3"/>
       <c r="J217" s="3"/>
@@ -13883,17 +13912,17 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>1218</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="C218" s="2" t="s">
         <v>1219</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D218" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E218:Z218),")")</f>
-        <v>(UT SAN ANTONIO|UTSA|TEXASSAN|UTS|TSA)</v>
+        <v>(TENN MARTIN|UTM|TENNMARTIN)</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>1220</v>
@@ -13904,12 +13933,8 @@
       <c r="G218" s="3" t="s">
         <v>1222</v>
       </c>
-      <c r="H218" s="3" t="s">
-        <v>1223</v>
-      </c>
-      <c r="I218" s="3" t="s">
-        <v>1224</v>
-      </c>
+      <c r="H218" s="3"/>
+      <c r="I218" s="3"/>
       <c r="J218" s="3"/>
       <c r="K218" s="3"/>
       <c r="L218" s="3"/>
@@ -13930,31 +13955,33 @@
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>351</v>
+        <v>1224</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>1226</v>
+        <v>101</v>
       </c>
       <c r="D219" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E219:Z219),")")</f>
-        <v>(UTAH|Utah|UTA|UTE)</v>
+        <v>(UT SAN ANTONIO|UTSA|TEXASSAN|UTS|TSA)</v>
       </c>
       <c r="E219" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F219" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G219" s="3" t="s">
         <v>1227</v>
       </c>
-      <c r="F219" s="0" t="s">
-        <v>1225</v>
-      </c>
-      <c r="G219" s="3" t="s">
+      <c r="H219" s="3" t="s">
         <v>1228</v>
       </c>
-      <c r="H219" s="3" t="s">
+      <c r="I219" s="3" t="s">
         <v>1229</v>
       </c>
-      <c r="I219" s="3"/>
       <c r="J219" s="3"/>
       <c r="K219" s="3"/>
       <c r="L219" s="3"/>
@@ -13978,30 +14005,28 @@
         <v>1230</v>
       </c>
       <c r="B220" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C220" s="2" t="s">
         <v>1231</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D220" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E220:Z220),")")</f>
-        <v>(UTAH ST|UTAHST|USU|US|UthSt)</v>
+        <v>(UTAH|Utah|UTA|UTE)</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>1232</v>
       </c>
-      <c r="F220" s="3" t="s">
+      <c r="F220" s="0" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G220" s="3" t="s">
         <v>1233</v>
       </c>
-      <c r="G220" s="3" t="s">
+      <c r="H220" s="3" t="s">
         <v>1234</v>
       </c>
-      <c r="H220" s="3" t="s">
-        <v>1235</v>
-      </c>
-      <c r="I220" s="0" t="s">
-        <v>1236</v>
-      </c>
+      <c r="I220" s="3"/>
       <c r="J220" s="3"/>
       <c r="K220" s="3"/>
       <c r="L220" s="3"/>
@@ -14022,28 +14047,33 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>1239</v>
+        <v>13</v>
       </c>
       <c r="D221" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E221:Z221),")")</f>
-        <v>(UTU|UTAH TECH|Utah)</v>
+        <v>(UTAH ST|UTAHST|USU|US|UthSt)</v>
       </c>
       <c r="E221" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F221" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="G221" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="H221" s="3" t="s">
         <v>1240</v>
       </c>
-      <c r="F221" s="4" t="s">
+      <c r="I221" s="0" t="s">
         <v>1241</v>
       </c>
-      <c r="G221" s="3" t="s">
-        <v>1225</v>
-      </c>
-      <c r="H221" s="3"/>
       <c r="J221" s="3"/>
       <c r="K221" s="3"/>
       <c r="L221" s="3"/>
@@ -14067,26 +14097,25 @@
         <v>1242</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>1108</v>
+        <v>1243</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>19</v>
+        <v>1244</v>
       </c>
       <c r="D222" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E222:Z222),")")</f>
-        <v>(UTEP|TEP|UTE)</v>
+        <v>(UTU|UTAH TECH|Utah)</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>1242</v>
-      </c>
-      <c r="F222" s="3" t="s">
-        <v>1243</v>
+        <v>1245</v>
+      </c>
+      <c r="F222" s="4" t="s">
+        <v>1246</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="H222" s="3"/>
-      <c r="I222" s="3"/>
       <c r="J222" s="3"/>
       <c r="K222" s="3"/>
       <c r="L222" s="3"/>
@@ -14106,27 +14135,27 @@
       <c r="Z222" s="3"/>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="4" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B223" s="5" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C223" s="5" t="s">
-        <v>1246</v>
+      <c r="A223" s="0" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D223" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E223:Z223),")")</f>
-        <v>(VALPARAISO|Valpo|VAL)</v>
-      </c>
-      <c r="E223" s="4" t="s">
+        <v>(UTEP|TEP|UTE)</v>
+      </c>
+      <c r="E223" s="3" t="s">
         <v>1247</v>
       </c>
-      <c r="F223" s="4" t="s">
+      <c r="F223" s="3" t="s">
         <v>1248</v>
       </c>
       <c r="G223" s="3" t="s">
-        <v>1249</v>
+        <v>1234</v>
       </c>
       <c r="H223" s="3"/>
       <c r="I223" s="3"/>
@@ -14149,34 +14178,30 @@
       <c r="Z223" s="3"/>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
+      <c r="A224" s="4" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B224" s="5" t="s">
         <v>1250</v>
       </c>
-      <c r="B224" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C224" s="2" t="s">
+      <c r="C224" s="5" t="s">
         <v>1251</v>
       </c>
       <c r="D224" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E224:Z224),")")</f>
-        <v>(VANDERBILT|VANDY|Vandy|VAN|VU)</v>
-      </c>
-      <c r="E224" s="3" t="s">
+        <v>(VALPARAISO|Valpo|VAL)</v>
+      </c>
+      <c r="E224" s="4" t="s">
         <v>1252</v>
       </c>
-      <c r="F224" s="3" t="s">
+      <c r="F224" s="4" t="s">
         <v>1253</v>
       </c>
-      <c r="G224" s="0" t="s">
+      <c r="G224" s="3" t="s">
         <v>1254</v>
       </c>
-      <c r="H224" s="3" t="s">
-        <v>1255</v>
-      </c>
-      <c r="I224" s="3" t="s">
-        <v>1256</v>
-      </c>
+      <c r="H224" s="3"/>
+      <c r="I224" s="3"/>
       <c r="J224" s="3"/>
       <c r="K224" s="3"/>
       <c r="L224" s="3"/>
@@ -14197,27 +14222,33 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>709</v>
+        <v>38</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="D225" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E225:Z225),")")</f>
-        <v>(VILLANOVA|VU)</v>
+        <v>(VANDERBILT|VANDY|Vandy|VAN|VU)</v>
       </c>
       <c r="E225" s="3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G225" s="0" t="s">
         <v>1259</v>
       </c>
-      <c r="F225" s="3" t="s">
-        <v>1256</v>
-      </c>
-      <c r="G225" s="3"/>
-      <c r="H225" s="3"/>
-      <c r="I225" s="3"/>
+      <c r="H225" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="I225" s="3" t="s">
+        <v>1261</v>
+      </c>
       <c r="J225" s="3"/>
       <c r="K225" s="3"/>
       <c r="L225" s="3"/>
@@ -14238,30 +14269,26 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>1261</v>
+        <v>709</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D226" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E226:Z226),")")</f>
-        <v>(VIRGINIA|Virg|VA|UVA)</v>
+        <v>(VILLANOVA|VU)</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>1263</v>
-      </c>
-      <c r="F226" s="0" t="s">
         <v>1264</v>
       </c>
-      <c r="G226" s="3" t="s">
-        <v>1265</v>
-      </c>
-      <c r="H226" s="3" t="s">
-        <v>1266</v>
-      </c>
+      <c r="F226" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G226" s="3"/>
+      <c r="H226" s="3"/>
       <c r="I226" s="3"/>
       <c r="J226" s="3"/>
       <c r="K226" s="3"/>
@@ -14283,36 +14310,32 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C227" s="2" t="s">
         <v>1267</v>
-      </c>
-      <c r="B227" s="2" t="s">
-        <v>1268</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>1269</v>
       </c>
       <c r="D227" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E227:Z227),")")</f>
-        <v>(VIRGINIA TECH|VATECH|VTech|VT|VaT|VAT)</v>
+        <v>(VIRGINIA|Virg|VA|UVA)</v>
       </c>
       <c r="E227" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="F227" s="0" t="s">
+        <v>1269</v>
+      </c>
+      <c r="G227" s="3" t="s">
         <v>1270</v>
       </c>
-      <c r="F227" s="3" t="s">
+      <c r="H227" s="3" t="s">
         <v>1271</v>
       </c>
-      <c r="G227" s="0" t="s">
-        <v>1272</v>
-      </c>
-      <c r="H227" s="3" t="s">
-        <v>1273</v>
-      </c>
-      <c r="I227" s="3" t="s">
-        <v>1274</v>
-      </c>
-      <c r="J227" s="3" t="s">
-        <v>1275</v>
-      </c>
+      <c r="I227" s="3"/>
+      <c r="J227" s="3"/>
       <c r="K227" s="3"/>
       <c r="L227" s="3"/>
       <c r="M227" s="3"/>
@@ -14332,26 +14355,36 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>621</v>
+        <v>1274</v>
       </c>
       <c r="D228" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E228:Z228),")")</f>
-        <v>(VMI)</v>
+        <v>(VIRGINIA TECH|VATECH|VTech|VT|VaT|VAT)</v>
       </c>
       <c r="E228" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F228" s="3" t="s">
         <v>1276</v>
       </c>
-      <c r="F228" s="3"/>
-      <c r="G228" s="3"/>
-      <c r="H228" s="3"/>
-      <c r="I228" s="3"/>
-      <c r="J228" s="3"/>
+      <c r="G228" s="0" t="s">
+        <v>1277</v>
+      </c>
+      <c r="H228" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="I228" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="J228" s="3" t="s">
+        <v>1280</v>
+      </c>
       <c r="K228" s="3"/>
       <c r="L228" s="3"/>
       <c r="M228" s="3"/>
@@ -14371,24 +14404,22 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>1278</v>
+        <v>1281</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>1279</v>
+        <v>1282</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>1280</v>
+        <v>621</v>
       </c>
       <c r="D229" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E229:Z229),")")</f>
-        <v>(WAGNER|WAG)</v>
+        <v>(VMI)</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>1281</v>
       </c>
-      <c r="F229" s="3" t="s">
-        <v>1282</v>
-      </c>
+      <c r="F229" s="3"/>
       <c r="G229" s="3"/>
       <c r="H229" s="3"/>
       <c r="I229" s="3"/>
@@ -14418,24 +14449,20 @@
         <v>1284</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>38</v>
+        <v>1285</v>
       </c>
       <c r="D230" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E230:Z230),")")</f>
-        <v>(WAKE FOREST|WAKEFOREST|WFU|WF)</v>
+        <v>(WAGNER|WAG)</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="F230" s="3" t="s">
-        <v>1286</v>
-      </c>
-      <c r="G230" s="0" t="s">
         <v>1287</v>
       </c>
-      <c r="H230" s="3" t="s">
-        <v>1288</v>
-      </c>
+      <c r="G230" s="3"/>
+      <c r="H230" s="3"/>
       <c r="I230" s="3"/>
       <c r="J230" s="3"/>
       <c r="K230" s="3"/>
@@ -14457,36 +14484,32 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B231" s="2" t="s">
         <v>1289</v>
       </c>
-      <c r="B231" s="2" t="s">
-        <v>1290</v>
-      </c>
       <c r="C231" s="2" t="s">
-        <v>1291</v>
+        <v>38</v>
       </c>
       <c r="D231" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E231:Z231),")")</f>
-        <v>(WASHINGTON|WASH|Wash|UW|WAS|U W)</v>
+        <v>(WAKE FOREST|WAKEFOREST|WFU|WF)</v>
       </c>
       <c r="E231" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G231" s="0" t="s">
         <v>1292</v>
       </c>
-      <c r="F231" s="3" t="s">
+      <c r="H231" s="3" t="s">
         <v>1293</v>
       </c>
-      <c r="G231" s="0" t="s">
-        <v>1294</v>
-      </c>
-      <c r="H231" s="3" t="s">
-        <v>1295</v>
-      </c>
-      <c r="I231" s="3" t="s">
-        <v>1296</v>
-      </c>
-      <c r="J231" s="3" t="s">
-        <v>1297</v>
-      </c>
+      <c r="I231" s="3"/>
+      <c r="J231" s="3"/>
       <c r="K231" s="3"/>
       <c r="L231" s="3"/>
       <c r="M231" s="3"/>
@@ -14506,34 +14529,36 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="D232" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E232:Z232),")")</f>
-        <v>(WASHINGTON ST|WSU|WASHST|COU|WshSt)</v>
+        <v>(WASHINGTON|WASH|Wash|UW|WAS|U W)</v>
       </c>
       <c r="E232" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F232" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G232" s="0" t="s">
+        <v>1299</v>
+      </c>
+      <c r="H232" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="I232" s="3" t="s">
         <v>1301</v>
       </c>
-      <c r="F232" s="3" t="s">
+      <c r="J232" s="3" t="s">
         <v>1302</v>
       </c>
-      <c r="G232" s="3" t="s">
-        <v>1303</v>
-      </c>
-      <c r="H232" s="3" t="s">
-        <v>1304</v>
-      </c>
-      <c r="I232" s="3" t="s">
-        <v>1305</v>
-      </c>
-      <c r="J232" s="3"/>
       <c r="K232" s="3"/>
       <c r="L232" s="3"/>
       <c r="M232" s="3"/>
@@ -14553,32 +14578,32 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="D233" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E233:Z233),")")</f>
-        <v>(WEBER ST|WEBERST|WEBER|WSU|WebSt)</v>
+        <v>(WASHINGTON ST|WSU|WASHST|COU|WshSt)</v>
       </c>
       <c r="E233" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F233" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="G233" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="H233" s="3" t="s">
         <v>1309</v>
       </c>
-      <c r="F233" s="3" t="s">
+      <c r="I233" s="3" t="s">
         <v>1310</v>
-      </c>
-      <c r="G233" s="3" t="s">
-        <v>1311</v>
-      </c>
-      <c r="H233" s="3" t="s">
-        <v>1302</v>
-      </c>
-      <c r="I233" s="0" t="s">
-        <v>1312</v>
       </c>
       <c r="J233" s="3"/>
       <c r="K233" s="3"/>
@@ -14600,17 +14625,17 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C234" s="2" t="s">
         <v>1313</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>1043</v>
       </c>
       <c r="D234" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E234:Z234),")")</f>
-        <v>(WEST VIRGINIA|WESTVIR|WVU|WVirg)</v>
+        <v>(WEBER ST|WEBERST|WEBER|WSU|WebSt)</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>1314</v>
@@ -14622,9 +14647,11 @@
         <v>1316</v>
       </c>
       <c r="H234" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="I234" s="0" t="s">
         <v>1317</v>
       </c>
-      <c r="I234" s="3"/>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
       <c r="L234" s="3"/>
@@ -14648,30 +14675,28 @@
         <v>1318</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>1319</v>
+        <v>214</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>1320</v>
+        <v>1043</v>
       </c>
       <c r="D235" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E235:Z235),")")</f>
-        <v>(WESTERN CAROLINA|WESTCARLNA|WESTRN CAROLINA|WCaro|WCU)</v>
+        <v>(WEST VIRGINIA|WESTVIR|WVU|WVirg)</v>
       </c>
       <c r="E235" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>1320</v>
+      </c>
+      <c r="G235" s="3" t="s">
         <v>1321</v>
       </c>
-      <c r="F235" s="3" t="s">
+      <c r="H235" s="3" t="s">
         <v>1322</v>
       </c>
-      <c r="G235" s="3" t="s">
-        <v>1323</v>
-      </c>
-      <c r="H235" s="0" t="s">
-        <v>1324</v>
-      </c>
-      <c r="I235" s="3" t="s">
-        <v>1325</v>
-      </c>
+      <c r="I235" s="3"/>
       <c r="J235" s="3"/>
       <c r="K235" s="3"/>
       <c r="L235" s="3"/>
@@ -14692,27 +14717,33 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>56</v>
+        <v>1325</v>
       </c>
       <c r="D236" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E236:Z236),")")</f>
-        <v>(WESTRN ILLINOIS|WIU)</v>
+        <v>(WESTERN CAROLINA|WESTCARLNA|WESTRN CAROLINA|WCaro|WCU)</v>
       </c>
       <c r="E236" s="3" t="s">
+        <v>1326</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="G236" s="3" t="s">
         <v>1328</v>
       </c>
-      <c r="F236" s="3" t="s">
+      <c r="H236" s="0" t="s">
         <v>1329</v>
       </c>
-      <c r="G236" s="3"/>
-      <c r="H236" s="3"/>
-      <c r="I236" s="3"/>
+      <c r="I236" s="3" t="s">
+        <v>1330</v>
+      </c>
       <c r="J236" s="3"/>
       <c r="K236" s="3"/>
       <c r="L236" s="3"/>
@@ -14733,30 +14764,26 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>408</v>
+        <v>1332</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>1331</v>
+        <v>56</v>
       </c>
       <c r="D237" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E237:Z237),")")</f>
-        <v>(WESTRN KENTUCKY|WKU|WESTERNKY|WKent)</v>
+        <v>(WESTRN ILLINOIS|WIU)</v>
       </c>
       <c r="E237" s="3" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="F237" s="3" t="s">
-        <v>1333</v>
-      </c>
-      <c r="G237" s="3" t="s">
         <v>1334</v>
       </c>
-      <c r="H237" s="3" t="s">
-        <v>1335</v>
-      </c>
+      <c r="G237" s="3"/>
+      <c r="H237" s="3"/>
       <c r="I237" s="3"/>
       <c r="J237" s="3"/>
       <c r="K237" s="3"/>
@@ -14778,33 +14805,31 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C238" s="2" t="s">
         <v>1336</v>
-      </c>
-      <c r="B238" s="2" t="s">
-        <v>1337</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>1338</v>
       </c>
       <c r="D238" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E238:Z238),")")</f>
-        <v>(WESTMICH|WESTRN MICHIGAN|WMU|WMich|WMI)</v>
+        <v>(WESTRN KENTUCKY|WKU|WESTERNKY|WKent)</v>
       </c>
       <c r="E238" s="3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="G238" s="3" t="s">
         <v>1339</v>
       </c>
-      <c r="F238" s="3" t="s">
+      <c r="H238" s="3" t="s">
         <v>1340</v>
       </c>
-      <c r="G238" s="3" t="s">
-        <v>1341</v>
-      </c>
-      <c r="H238" s="0" t="s">
-        <v>1342</v>
-      </c>
-      <c r="I238" s="3" t="s">
-        <v>1343</v>
-      </c>
+      <c r="I238" s="3"/>
       <c r="J238" s="3"/>
       <c r="K238" s="3"/>
       <c r="L238" s="3"/>
@@ -14825,29 +14850,33 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="D239" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E239:Z239),")")</f>
-        <v>(MARY|WILLMMARY|WM)</v>
+        <v>(WESTMICH|WESTRN MICHIGAN|WMU|WMich|WMI)</v>
       </c>
       <c r="E239" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F239" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="H239" s="0" t="s">
         <v>1347</v>
       </c>
-      <c r="F239" s="0" t="s">
+      <c r="I239" s="3" t="s">
         <v>1348</v>
       </c>
-      <c r="G239" s="3" t="s">
-        <v>1349</v>
-      </c>
-      <c r="H239" s="3"/>
-      <c r="I239" s="3"/>
       <c r="J239" s="3"/>
       <c r="K239" s="3"/>
       <c r="L239" s="3"/>
@@ -14868,17 +14897,17 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B240" s="2" t="s">
         <v>1350</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="C240" s="2" t="s">
         <v>1351</v>
-      </c>
-      <c r="C240" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D240" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E240:Z240),")")</f>
-        <v>(WISCONSIN|Wisc|WIS)</v>
+        <v>(MARY|WILLMMARY|WM)</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>1352</v>
@@ -14921,15 +14950,17 @@
       </c>
       <c r="D241" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E241:Z241),")")</f>
-        <v>(WOFFORD|WOF)</v>
+        <v>(WISCONSIN|Wisc|WIS)</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>1357</v>
       </c>
-      <c r="F241" s="3" t="s">
+      <c r="F241" s="0" t="s">
         <v>1358</v>
       </c>
-      <c r="G241" s="3"/>
+      <c r="G241" s="3" t="s">
+        <v>1359</v>
+      </c>
       <c r="H241" s="3"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3"/>
@@ -14952,30 +14983,27 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>1361</v>
+        <v>32</v>
       </c>
       <c r="D242" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E242:Z242),")")</f>
-        <v>(WYOMING|Wyom|WYO|WY)</v>
+        <v>(WOFFORD|WOF)</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>1362</v>
       </c>
-      <c r="F242" s="0" t="s">
+      <c r="F242" s="3" t="s">
         <v>1363</v>
       </c>
-      <c r="G242" s="3" t="s">
-        <v>1364</v>
-      </c>
-      <c r="H242" s="3" t="s">
-        <v>1365</v>
-      </c>
+      <c r="G242" s="3"/>
+      <c r="H242" s="3"/>
+      <c r="I242" s="3"/>
       <c r="J242" s="3"/>
       <c r="K242" s="3"/>
       <c r="L242" s="3"/>
@@ -14996,27 +15024,30 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C243" s="2" t="s">
         <v>1366</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>1367</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D243" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E243:Z243),")")</f>
-        <v>(YALE|YAL)</v>
+        <v>(WYOMING|Wyom|WYO|WY)</v>
       </c>
       <c r="E243" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="F243" s="0" t="s">
         <v>1368</v>
       </c>
-      <c r="F243" s="3" t="s">
+      <c r="G243" s="3" t="s">
         <v>1369</v>
       </c>
-      <c r="G243" s="3"/>
-      <c r="H243" s="3"/>
-      <c r="I243" s="3"/>
+      <c r="H243" s="3" t="s">
+        <v>1370</v>
+      </c>
       <c r="J243" s="3"/>
       <c r="K243" s="3"/>
       <c r="L243" s="3"/>
@@ -15037,27 +15068,25 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>442</v>
+        <v>1372</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>1371</v>
+        <v>32</v>
       </c>
       <c r="D244" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E244:Z244),")")</f>
-        <v>(YOUNGSTOWN ST|YSU|YngSt)</v>
+        <v>(YALE|YAL)</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="F244" s="3" t="s">
-        <v>1373</v>
-      </c>
-      <c r="G244" s="3" t="s">
         <v>1374</v>
       </c>
+      <c r="G244" s="3"/>
       <c r="H244" s="3"/>
       <c r="I244" s="3"/>
       <c r="J244" s="3"/>
@@ -15079,9 +15108,28 @@
       <c r="Z244" s="3"/>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E245" s="3"/>
-      <c r="F245" s="3"/>
-      <c r="G245" s="3"/>
+      <c r="A245" s="0" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D245" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("(",_xlfn.TEXTJOIN("|",TRUE(),E245:Z245),")")</f>
+        <v>(YOUNGSTOWN ST|YSU|YngSt)</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G245" s="3" t="s">
+        <v>1379</v>
+      </c>
       <c r="H245" s="3"/>
       <c r="I245" s="3"/>
       <c r="J245" s="3"/>
@@ -15222,14 +15270,38 @@
       <c r="Y250" s="3"/>
       <c r="Z250" s="3"/>
     </row>
+    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="3"/>
+      <c r="H251" s="3"/>
+      <c r="I251" s="3"/>
+      <c r="J251" s="3"/>
+      <c r="K251" s="3"/>
+      <c r="L251" s="3"/>
+      <c r="M251" s="3"/>
+      <c r="N251" s="3"/>
+      <c r="O251" s="3"/>
+      <c r="P251" s="3"/>
+      <c r="Q251" s="3"/>
+      <c r="R251" s="3"/>
+      <c r="S251" s="3"/>
+      <c r="T251" s="3"/>
+      <c r="U251" s="3"/>
+      <c r="V251" s="3"/>
+      <c r="W251" s="3"/>
+      <c r="X251" s="3"/>
+      <c r="Y251" s="3"/>
+      <c r="Z251" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A222:A1048576 A77:A192 A1:A75 A194:A220">
+  <conditionalFormatting sqref="A223:A1048576 A77:A192 A1:A75 A202:A221 A194:A200">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E216:Z218 G219:Z219 E219 E222:Z222 E220:H220 J220:Z221 E225:Z225 E228:Z229 E227:F227 H227:Z227 G226:Z226 E226 E224:F224 H224:Z224 E234:Z234 E236:Z237 E238:G238 I238:Z238 E235:G235 I235:Z235 E233:H233 J233:Z233 E243:Z250 J242:Z242 E242 G242:H242 E232:Z232 H230:Z231 E230:F231 G215:Z215 E215 E241:Z241 G239:Z240 E239:E240 E221 G221:H221 F223:Z223">
+  <conditionalFormatting sqref="E217:Z219 G220:Z220 E220 E223:Z223 E221:H221 J221:Z222 E226:Z226 E229:Z230 E228:F228 H228:Z228 G227:Z227 E227 E225:F225 H225:Z225 E235:Z235 E237:Z238 E239:G239 I239:Z239 E236:G236 I236:Z236 E234:H234 J234:Z234 E244:Z251 J243:Z243 E243 G243:H243 E233:Z233 H231:Z232 E231:F232 G216:Z216 E216 E242:Z242 G240:Z241 E240:E241 E222 G222:H222 F224:Z224">
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I109 H100:J100 J124:Z124 E124:H124 E125:Z125 G127:Z127 I126:Z126 F126:G126 E2:Z2 E58:Z58 E56:F57 H56:Z56 K57:Z57 G57:I57 E59:H59 J59:Z59 E60:Z62 H64:Z64 E64:F64 F65:Z66 E65:E70 F72:Z73 I70:Z70 F70:G70 H71:Z71 E71:F71 E72:E74 E75:Z76 J74:Z74 F74:H74 E79:Z79 E81:Z89 G80:Z80 E80 K91:Z91 H91:I91 L90:Z90 G90:J90 E77:G77 I77:Z77 E96:Z99 H95:Z95 E94:F95 E103:Z104 K102:Z102 E102:I102 I101:Z101 E107:Z107 H106:Z106 E106:F106 E108:E109 E110:Z110 E113:Z114 E112:G112 I112:Z112 E111:H111 J111:Z111 E118:Z118 E120:Z122 E123:F123 H123:Z123 J119:Z119 E119:H119 E115:G116 J115:Z116 J117:K117 M117:Z117 E116:H117 E130:Z130 K131:Z131 E131:I131 G129:I129 K129:Z129 E128:F129 H128:Z128 E134:Z137 E139:Z145 G138:Z138 E138 E132:G132 F152:Z153 J151:Z151 F151:H151 L150:Z150 F150:J150 G149:H149 J149:Z149 F156:Z161 I155:Z155 F155:G155 L154:Z154 F154:J154 E146:I146 L146:Z146 E166:Z166 I168:Z168 J167:Z167 E165:G165 I165:Z165 E169:Z171 E168:G168 E167:H167 E174:Z176 E173:F173 H173:Z173 E179:Z180 E183:Z183 J182:Z182 E182:H182 E177:F178 E172:G172 I172:K172 N172:Z172 E185:Z188 J184:Z184 E184:H184 E189 G189:I189 K189:Z189 E197:Z197 G198:Z199 G195:Z195 J196:Z196 F196:H196 E195:E196 E201:Z201 E198:E199 E200:F200 H200:Z200 E203:Z203 E202:F202 H202:Z202 E208:Z208 E210:Z210 E212:Z213 E214:F214 H214:Z214 G211:Z211 E211 G209:Z209 E209 E207:G207 I207:Z207 E3:H3 J3:Z3 I115 E4:Z4 E10:F10 I10:Z10 E92:Z93 E90:F91 E23 G23:Z23 E147:E162 E163:Z163 G162:Z162 F105:Z105 E206:Z206 E204:F204 E205 G205 H204:Z204 I205:Z205 E126:E127 F68:Z68 L69:Z69 F69:J69 F67:G67 I67:Z67 E50:Z53 E55:Z55 E54:F54 H54:Z54 E48 G48:Z48 E101:G101 N100:Z100 L100 E100:F100 J78:Z78 E78:F78 H78 F190:Z190 J108:Z108 K109:Z109 F109 G108:H108 K147:Z147 H147:I147 F147:F149 E133:I133 K133:Z133 F49:Z49 E37:Z37 E39:F40 H39:Z40 G38:Z38 E38 E36 G36:Z36 L148:Z148 H148:J148 E63:G63 I63:Z63 J94:Z94 G94:H94 E11:Z11 E13:Z13 E12:F12 H12:Z12 E15:Z15 G16:Z16 E16 E14:F14 H14:Z14 E164 G164:Z164 E191:Z194 E6:Z9 E5 L132:Z132 I132:J132 E18:Z18 E20:Z21 E22:F22 H22:Z22 E19:G19 I19:Z19 E17:F17 H17:Z17 E24:Z28 E30:Z33 G29:Z29 E29 E35:Z35 E34:F34 H34:Z34 E41:Z42 E45:Z47 H43:Z44 E43:F44 H177:Z178 G5:Z5 E181:F181 H181:Z181">
+  <conditionalFormatting sqref="I109 H100:J100 J124:Z124 E124:H124 E125:Z125 G127:Z127 I126:Z126 F126:G126 E2:Z2 E58:Z58 E56:F57 H56:Z56 K57:Z57 G57:I57 E59:H59 J59:Z59 E60:Z62 H64:Z64 E64:F64 F65:Z66 E65:E70 F72:Z73 I70:Z70 F70:G70 H71:Z71 E71:F71 E72:E74 E75:Z76 J74:Z74 F74:H74 E79:Z79 E81:Z89 G80:Z80 E80 K91:Z91 H91:I91 L90:Z90 G90:J90 E77:G77 I77:Z77 E96:Z99 H95:Z95 E94:F95 E103:Z104 K102:Z102 E102:I102 I101:Z101 E107:Z107 H106:Z106 E106:F106 E108:E109 E110:Z110 E113:Z114 E112:G112 I112:Z112 E111:H111 J111:Z111 E118:Z118 E120:Z122 E123:F123 H123:Z123 J119:Z119 E119:H119 E115:G116 J115:Z116 J117:K117 M117:Z117 E116:H117 E130:Z130 K131:Z131 E131:I131 G129:I129 K129:Z129 E128:F129 H128:Z128 E134:Z137 E139:Z145 G138:Z138 E138 E132:G132 F152:Z153 J151:Z151 F151:H151 L150:Z150 F150:J150 G149:H149 J149:Z149 F156:Z161 I155:Z155 F155:G155 L154:Z154 F154:J154 E146:I146 L146:Z146 E166:Z166 I168:Z168 J167:Z167 E165:G165 I165:Z165 E169:Z171 E168:G168 E167:H167 E174:Z176 E173:F173 H173:Z173 E179:Z180 E183:Z183 J182:Z182 E182:H182 E177:F178 E172:G172 I172:K172 N172:Z172 E185:Z188 J184:Z184 E184:H184 E189 G189:I189 K189:Z189 E197:Z197 G198:Z199 G195:Z195 J196:Z196 F196:H196 E195:E196 E202:Z202 E198:E199 E200:F200 H200:Z201 E204:Z204 E203:F203 H203:Z203 E209:Z209 E211:Z211 E213:Z214 E215:F215 H215:Z215 G212:Z212 E212 G210:Z210 E210 E208:G208 I208:Z208 E3:H3 J3:Z3 I115 E4:Z4 E10:F10 I10:Z10 E92:Z93 E90:F91 E23 G23:Z23 E147:E162 E163:Z163 G162:Z162 F105:Z105 E207:Z207 E205:F205 E206 G206 H205:Z205 I206:Z206 E126:E127 F68:Z68 L69:Z69 F69:J69 F67:G67 I67:Z67 E50:Z53 E55:Z55 E54:F54 H54:Z54 E48 G48:Z48 E101:G101 N100:Z100 L100 E100:F100 J78:Z78 E78:F78 H78 F190:Z190 J108:Z108 K109:Z109 F109 G108:H108 K147:Z147 H147:I147 F147:F149 E133:I133 K133:Z133 F49:Z49 E37:Z37 E39:F40 H39:Z40 G38:Z38 E38 E36 G36:Z36 L148:Z148 H148:J148 E63:G63 I63:Z63 J94:Z94 G94:H94 E11:Z11 E13:Z13 E12:F12 H12:Z12 E15:Z15 G16:Z16 E16 E14:F14 H14:Z14 E164 G164:Z164 E191:Z194 E6:Z9 E5 L132:Z132 I132:J132 E18:Z18 E20:Z21 E22:F22 H22:Z22 E19:G19 I19:Z19 E17:F17 H17:Z17 E24:Z28 E30:Z33 G29:Z29 E29 E35:Z35 E34:F34 H34:Z34 E41:Z42 E45:Z47 H43:Z44 E43:F44 H177:Z178 G5:Z5 E181:F181 H181:Z181 E201">
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>